<commit_message>
PortfolioView replacement elements, Issue# 37
This includes a change to fix issue with unquoted numbers Issue# 37,  as well as a lot of element fixes to smf-elements-6 & 9.  Zacks and Barchart items.
</commit_message>
<xml_diff>
--- a/docs/samples/PortfolioView replacement items.xlsx
+++ b/docs/samples/PortfolioView replacement items.xlsx
@@ -867,8 +867,8 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update PortfolioView replacement items.xlsx
</commit_message>
<xml_diff>
--- a/docs/samples/PortfolioView replacement items.xlsx
+++ b/docs/samples/PortfolioView replacement items.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="147">
   <si>
     <t>Symbol</t>
   </si>
@@ -447,13 +447,22 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>smfUnix2Date(smfStrExtr(s1, """date"":", ","))</t>
-  </si>
-  <si>
     <t>Can't find</t>
   </si>
   <si>
     <t>No data to return</t>
+  </si>
+  <si>
+    <t>=smfUnix2Date(D77)</t>
+  </si>
+  <si>
+    <t>=smfUnix2DateStr(D77,"HH:MM")</t>
+  </si>
+  <si>
+    <t>Error is due to the Unix2DateStr running on empty data</t>
+  </si>
+  <si>
+    <t>No post market data during trading day</t>
   </si>
 </sst>
 </file>
@@ -562,7 +571,6 @@
     </sheetNames>
     <definedNames>
       <definedName name="RCHGetElementNumber"/>
-      <definedName name="smfGetYahooJSONData"/>
       <definedName name="smfUnix2Date"/>
       <definedName name="smfUnix2DateStr"/>
     </definedNames>
@@ -866,18 +874,18 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
+      <pane ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" customWidth="1"/>
-    <col min="6" max="6" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" customWidth="1"/>
+    <col min="6" max="6" width="76" customWidth="1"/>
     <col min="7" max="7" width="35.140625" customWidth="1"/>
     <col min="8" max="8" width="34.28515625" customWidth="1"/>
   </cols>
@@ -898,7 +906,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>90</v>
       </c>
@@ -1062,7 +1070,7 @@
       </c>
       <c r="D11" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A11)</f>
-        <v>POSTPOST</v>
+        <v>REGULAR</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="str">
@@ -1238,7 +1246,7 @@
       </c>
       <c r="D19" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A19)</f>
-        <v>179.58</v>
+        <v>178.49</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="str">
@@ -1260,7 +1268,7 @@
       </c>
       <c r="D20" s="13">
         <f>[1]!RCHGetElementNumber(ticker,A20)</f>
-        <v>1685995205</v>
+        <v>1686156405</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="str">
@@ -1282,7 +1290,7 @@
       </c>
       <c r="D21" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A21)</f>
-        <v>-1.3699950999999999</v>
+        <v>-0.72000120000000001</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="str">
@@ -1304,12 +1312,12 @@
       </c>
       <c r="D22" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A22)</f>
-        <v>182.63</v>
+        <v>178.44</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A22)</f>
-        <v>=smfGetYahooJSONData(ticker,"price","regularMarketOpen")</v>
+        <v>=smfGetYahooJSONData("~~~~~","price","regularMarketOpen")</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1326,12 +1334,12 @@
       </c>
       <c r="D23" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A23)</f>
-        <v>184.95</v>
+        <v>181.21</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A23)</f>
-        <v>=smfGetYahooJSONData(ticker,"price","regularMarketDayHigh")</v>
+        <v>=smfGetYahooJSONData("~~~~~","price","regularMarketDayHigh")</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,12 +1356,12 @@
       </c>
       <c r="D24" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A24)</f>
-        <v>178.035</v>
+        <v>178.18</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A24)</f>
-        <v>=smfGetYahooJSONData(ticker,"price","regularMarketDayLow")</v>
+        <v>=smfGetYahooJSONData("~~~~~","price","regularMarketDayLow")</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,12 +1378,12 @@
       </c>
       <c r="D25" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A25)</f>
-        <v>119267468</v>
+        <v>29598912</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A25)</f>
-        <v>=smfGetYahooJSONData(ticker,"price","regularMarketVolume")</v>
+        <v>=smfGetYahooJSONData("~~~~~","price","regularMarketVolume")</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,7 +1400,7 @@
       </c>
       <c r="D26" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A26)</f>
-        <v>179.3</v>
+        <v>178.48</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="str">
@@ -1414,7 +1422,7 @@
       </c>
       <c r="D27" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A27)</f>
-        <v>179.13</v>
+        <v>178.49</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="str">
@@ -1458,7 +1466,7 @@
       </c>
       <c r="D29" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A29)</f>
-        <v>2824559919104</v>
+        <v>2807415701504</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="str">
@@ -1483,7 +1491,7 @@
         <v>Not defined yet</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F30" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A30)</f>
@@ -1504,12 +1512,12 @@
       </c>
       <c r="D31" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A31)</f>
-        <v>180.8</v>
+        <v>185.74</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A31)</f>
-        <v>=smfGetYahooJSONData(ticker,"financialData","targetMeanPrice")</v>
+        <v>=smfGetYahooJSONData("~~~~~","financialData","targetMeanPrice")</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,7 +1539,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A32)</f>
-        <v>=smfGetYahooJSONData(ticker,"financialData","totalRevenue")</v>
+        <v>=smfGetYahooJSONData("~~~~~","financialData","totalRevenue")</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1548,7 +1556,7 @@
       </c>
       <c r="D33" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A33)</f>
-        <v>7.3347090000000001</v>
+        <v>7.2901897</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="str">
@@ -1570,7 +1578,7 @@
       </c>
       <c r="D34" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A34)</f>
-        <v>30.232323000000001</v>
+        <v>30.048822000000001</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="str">
@@ -1724,7 +1732,7 @@
       </c>
       <c r="D41" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A41)</f>
-        <v>5.0842776000000001E-3</v>
+        <v>5.1336419999999999E-3</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="str">
@@ -1812,7 +1820,7 @@
       </c>
       <c r="D45" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A45)</f>
-        <v>45.428787</v>
+        <v>45.15305</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="str">
@@ -1856,7 +1864,7 @@
       </c>
       <c r="D47" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A47)</f>
-        <v>3.78</v>
+        <v>3.77</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="str">
@@ -1878,7 +1886,7 @@
       </c>
       <c r="D48" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A48)</f>
-        <v>27.375</v>
+        <v>27.208843000000002</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="str">
@@ -1905,7 +1913,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A49)</f>
-        <v>=smfGetYahooJSONData(ticker,"financialData","ebitda")</v>
+        <v>=smfGetYahooJSONData("~~~~~","financialData","ebitda")</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1988,7 +1996,7 @@
       </c>
       <c r="D53" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A53)</f>
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="str">
@@ -2010,7 +2018,7 @@
       </c>
       <c r="D54" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A54)</f>
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="str">
@@ -2032,7 +2040,7 @@
       </c>
       <c r="D55" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A55)</f>
-        <v>180.95</v>
+        <v>179.21</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="str">
@@ -2054,7 +2062,7 @@
       </c>
       <c r="D56" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A56)</f>
-        <v>-7.5711253999999999E-3</v>
+        <v>-4.0176394000000001E-3</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="str">
@@ -2076,11 +2084,11 @@
       </c>
       <c r="D57" s="8">
         <f>[1]!RCHGetElementNumber(ticker,A57)</f>
-        <v>-1.3699950999999999</v>
+        <v>-0.72000120000000001</v>
       </c>
       <c r="E57" s="2">
         <f>D23-D24</f>
-        <v>6.914999999999992</v>
+        <v>3.0300000000000011</v>
       </c>
       <c r="F57" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A57)</f>
@@ -2104,7 +2112,7 @@
         <v>Not found</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F58" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A58)</f>
@@ -2147,7 +2155,7 @@
       </c>
       <c r="D60" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A60)</f>
-        <v>168.35499999999999</v>
+        <v>169.1472</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="str">
@@ -2213,7 +2221,7 @@
       </c>
       <c r="D63" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A63)</f>
-        <v>152.46475000000001</v>
+        <v>152.51519999999999</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2" t="str">
@@ -2279,7 +2287,7 @@
       </c>
       <c r="D66" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A66)</f>
-        <v>0.21679783</v>
+        <v>0.21120572000000001</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2" t="str">
@@ -2431,11 +2439,13 @@
         <f>[1]!RCHGetElementNumber("Element",A73)</f>
         <v>Post-Mkt Time (UNIX)</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A73)</f>
-        <v>1686009599</v>
-      </c>
-      <c r="E73" s="2"/>
+        <v>Not found</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="F73" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A73)</f>
         <v>=smfGetYahooJSONData("~~~~~","price","postMarketTime",,"num")</v>
@@ -2453,9 +2463,9 @@
         <f>[1]!RCHGetElementNumber("Element",A74)</f>
         <v>Post Mkt Price</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D74" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A74)</f>
-        <v>179.08500000000001</v>
+        <v>Not found</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2" t="str">
@@ -2475,9 +2485,9 @@
         <f>[1]!RCHGetElementNumber("Element",A75)</f>
         <v>Post Mkt Chg</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A75)</f>
-        <v>-0.49499500000000002</v>
+        <v>Not found</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="str">
@@ -2497,9 +2507,9 @@
         <f>[1]!RCHGetElementNumber("Element",A76)</f>
         <v>Post Mkt Chg%</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A76)</f>
-        <v>-2.7564E-3</v>
+        <v>Not found</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="str">
@@ -2521,7 +2531,7 @@
       </c>
       <c r="D77" s="2">
         <f>[1]!RCHGetElementNumber(ticker,A77)</f>
-        <v>1685971799</v>
+        <v>1686144598</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="str">
@@ -2543,7 +2553,7 @@
       </c>
       <c r="D78" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A78)</f>
-        <v>182.56700000000001</v>
+        <v>178.3</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="str">
@@ -2565,7 +2575,7 @@
       </c>
       <c r="D79" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A79)</f>
-        <v>1.617</v>
+        <v>-0.91000400000000004</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="str">
@@ -2587,7 +2597,7 @@
       </c>
       <c r="D80" s="5">
         <f>[1]!RCHGetElementNumber(ticker,A80)</f>
-        <v>8.9361900000000001E-3</v>
+        <v>-5.07786E-3</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="str">
@@ -2633,7 +2643,7 @@
       </c>
       <c r="D82" s="8" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A82)</f>
-        <v>2023-06-05</v>
+        <v>2023-06-07</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2" t="str">
@@ -2655,7 +2665,7 @@
       </c>
       <c r="D83" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A83)</f>
-        <v>20:00</v>
+        <v>16:46</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="str">
@@ -2743,9 +2753,11 @@
       </c>
       <c r="D87" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A87)</f>
-        <v>2023-06-05</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>Error</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F87" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A87)</f>
         <v>=smfUnix2DateStr(smfGetYahooJSONData("~~~~~","price","postMarketTime",,"num"))</v>
@@ -2765,9 +2777,11 @@
       </c>
       <c r="D88" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A88)</f>
-        <v>23:59</v>
-      </c>
-      <c r="E88" s="2"/>
+        <v>Error</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F88" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A88)</f>
         <v>==smfUnix2DateStr(smfGetYahooJSONData("~~~~~","price","postMarketTime",,"num"),"HH:MM")</v>
@@ -2787,7 +2801,7 @@
       </c>
       <c r="D89" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A89)</f>
-        <v>2023-06-05</v>
+        <v>2023-06-07</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="str">
@@ -2831,7 +2845,7 @@
       </c>
       <c r="D91" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A91)</f>
-        <v>2023-06-05 20:00</v>
+        <v>2023-06-07 16:46</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="str">
@@ -2853,9 +2867,11 @@
       </c>
       <c r="D92" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A92)</f>
-        <v>2023-06-05 23:59</v>
-      </c>
-      <c r="E92" s="2"/>
+        <v>Error</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F92" s="2" t="str">
         <f>[1]!RCHGetElementNumber("Web Page",A92)</f>
         <v>=smfUnix2DateStr(smfGetYahooJSONData("~~~~~","price","postMarketTime",,"num"),"yyyy-mm-dd HH:MM")</v>
@@ -2875,7 +2891,7 @@
       </c>
       <c r="D93" s="5" t="str">
         <f>[1]!RCHGetElementNumber(ticker,A93)</f>
-        <v>2023-06-05 13:29</v>
+        <v>2023-06-07 13:29</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="str">
@@ -2927,25 +2943,24 @@
         <v>="Not defined yet"</v>
       </c>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F97" t="str">
-        <f>[1]!smfGetYahooJSONData("ticker","price","preMarketTime")</f>
-        <v>Not found</v>
-      </c>
-    </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F99" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F100" s="12">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="9"/>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C100" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D100" s="12">
         <f>[1]!smfUnix2Date(D77)</f>
-        <v>45082.56248842593</v>
-      </c>
-    </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F101" t="str">
+        <v>45084.562476851846</v>
+      </c>
+      <c r="F100" s="12"/>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D101" s="5" t="str">
         <f>[1]!smfUnix2DateStr(D77,"HH:MM")</f>
         <v>13:29</v>
       </c>

</xml_diff>